<commit_message>
starting trial for abstract class and sub-class using static methods. sex-age template works. need for ui setup
</commit_message>
<xml_diff>
--- a/data/raw/population/age-sex-maritial-status/population-age-sex-maritial_status-district-2018-elazığ-konya.xlsx
+++ b/data/raw/population/age-sex-maritial-status/population-age-sex-maritial_status-district-2018-elazığ-konya.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\tartan-analytics\data\raw\population\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\tartan-analytics\data\raw\population\age-sex-maritial-status\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13155" windowHeight="7140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -1206,9 +1206,6 @@
     <t>Kilis(Polateli)-2025</t>
   </si>
   <si>
-    <t>Kırıkkale(Bahşili)-1880</t>
-  </si>
-  <si>
     <t>Kırıkkale(Balışeyh)-1882</t>
   </si>
   <si>
@@ -1405,6 +1402,9 @@
   </si>
   <si>
     <t>Konya(Yunak)-1735</t>
+  </si>
+  <si>
+    <t>Kırıkkale(Bahşılı)-1880</t>
   </si>
 </sst>
 </file>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EA335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="C268" sqref="C268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -95026,7 +95026,7 @@
     <row r="268" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="B268" t="s">
-        <v>395</v>
+        <v>461</v>
       </c>
       <c r="F268">
         <v>281</v>
@@ -95353,7 +95353,7 @@
     <row r="269" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="B269" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F269">
         <v>266</v>
@@ -95677,7 +95677,7 @@
     <row r="270" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="B270" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F270">
         <v>89</v>
@@ -95983,7 +95983,7 @@
     <row r="271" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="B271" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -96325,7 +96325,7 @@
     <row r="272" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="B272" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F272">
         <v>178</v>
@@ -96613,7 +96613,7 @@
     <row r="273" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="B273" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E273">
         <v>2</v>
@@ -96958,7 +96958,7 @@
     <row r="274" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="B274" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E274">
         <v>22</v>
@@ -97336,7 +97336,7 @@
     <row r="275" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="B275" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -97687,7 +97687,7 @@
     <row r="276" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="B276" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -98023,7 +98023,7 @@
     <row r="277" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1"/>
       <c r="B277" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E277">
         <v>12</v>
@@ -98383,7 +98383,7 @@
     <row r="278" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="B278" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -98725,7 +98725,7 @@
     <row r="279" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="B279" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F279">
         <v>43</v>
@@ -99019,7 +99019,7 @@
     <row r="280" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="B280" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -99394,7 +99394,7 @@
     <row r="281" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="B281" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E281">
         <v>23</v>
@@ -99763,7 +99763,7 @@
     <row r="282" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1"/>
       <c r="B282" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -100084,7 +100084,7 @@
     <row r="283" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="B283" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -100432,7 +100432,7 @@
     <row r="284" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1"/>
       <c r="B284" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E284">
         <v>7</v>
@@ -100789,7 +100789,7 @@
     <row r="285" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1"/>
       <c r="B285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F285">
         <v>140</v>
@@ -101095,7 +101095,7 @@
     <row r="286" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1"/>
       <c r="B286" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F286">
         <v>264</v>
@@ -101422,7 +101422,7 @@
     <row r="287" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="B287" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F287">
         <v>184</v>
@@ -101749,7 +101749,7 @@
     <row r="288" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1"/>
       <c r="B288" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -102088,7 +102088,7 @@
     <row r="289" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1"/>
       <c r="B289" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E289">
         <v>5</v>
@@ -102454,7 +102454,7 @@
     <row r="290" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="B290" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E290">
         <v>11</v>
@@ -102829,7 +102829,7 @@
     <row r="291" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="B291" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E291">
         <v>2</v>
@@ -103183,7 +103183,7 @@
     <row r="292" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="B292" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E292">
         <v>4</v>
@@ -103552,7 +103552,7 @@
     <row r="293" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="B293" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E293">
         <v>12</v>
@@ -103912,7 +103912,7 @@
     <row r="294" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="B294" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E294">
         <v>15</v>
@@ -104287,7 +104287,7 @@
     <row r="295" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="B295" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E295">
         <v>11</v>
@@ -104665,7 +104665,7 @@
     <row r="296" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="B296" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E296">
         <v>6</v>
@@ -105025,7 +105025,7 @@
     <row r="297" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="B297" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C297">
         <v>2</v>
@@ -105406,7 +105406,7 @@
     <row r="298" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="B298" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E298">
         <v>11</v>
@@ -105778,7 +105778,7 @@
     <row r="299" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E299">
         <v>56</v>
@@ -106156,7 +106156,7 @@
     <row r="300" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="B300" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E300">
         <v>12</v>
@@ -106525,7 +106525,7 @@
     <row r="301" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="B301" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E301">
         <v>4</v>
@@ -106891,7 +106891,7 @@
     <row r="302" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="B302" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E302">
         <v>7</v>
@@ -107263,7 +107263,7 @@
     <row r="303" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="B303" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E303">
         <v>13</v>
@@ -107638,7 +107638,7 @@
     <row r="304" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="B304" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E304">
         <v>2</v>
@@ -107953,7 +107953,7 @@
     <row r="305" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="B305" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E305">
         <v>3</v>
@@ -108262,7 +108262,7 @@
     <row r="306" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="B306" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E306">
         <v>16</v>
@@ -108637,7 +108637,7 @@
     <row r="307" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="B307" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E307">
         <v>12</v>
@@ -108949,7 +108949,7 @@
     <row r="308" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1"/>
       <c r="B308" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E308">
         <v>16</v>
@@ -109315,7 +109315,7 @@
     <row r="309" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="1"/>
       <c r="B309" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E309">
         <v>3</v>
@@ -109669,7 +109669,7 @@
     <row r="310" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1"/>
       <c r="B310" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E310">
         <v>3</v>
@@ -109996,7 +109996,7 @@
     <row r="311" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="B311" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E311">
         <v>16</v>
@@ -110353,7 +110353,7 @@
     <row r="312" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="B312" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E312">
         <v>23</v>
@@ -110719,7 +110719,7 @@
     <row r="313" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="B313" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E313">
         <v>1</v>
@@ -111034,7 +111034,7 @@
     <row r="314" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="B314" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F314">
         <v>215</v>
@@ -111364,7 +111364,7 @@
     <row r="315" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="B315" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E315">
         <v>6</v>
@@ -111700,7 +111700,7 @@
     <row r="316" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="B316" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E316">
         <v>4</v>
@@ -112018,7 +112018,7 @@
     <row r="317" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
       <c r="B317" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E317">
         <v>21</v>
@@ -112396,7 +112396,7 @@
     <row r="318" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="B318" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E318">
         <v>2</v>
@@ -112717,7 +112717,7 @@
     <row r="319" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="B319" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E319">
         <v>4</v>
@@ -113056,7 +113056,7 @@
     <row r="320" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="B320" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F320">
         <v>178</v>
@@ -113359,7 +113359,7 @@
     <row r="321" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
       <c r="B321" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E321">
         <v>3</v>
@@ -113704,7 +113704,7 @@
     <row r="322" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1"/>
       <c r="B322" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E322">
         <v>15</v>
@@ -114073,7 +114073,7 @@
     <row r="323" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="1"/>
       <c r="B323" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E323">
         <v>19</v>
@@ -114424,7 +114424,7 @@
     <row r="324" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1"/>
       <c r="B324" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E324">
         <v>5</v>
@@ -114778,7 +114778,7 @@
     <row r="325" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="1"/>
       <c r="B325" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C325">
         <v>1</v>
@@ -115153,7 +115153,7 @@
     <row r="326" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1"/>
       <c r="B326" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E326">
         <v>20</v>
@@ -115510,7 +115510,7 @@
     <row r="327" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="1"/>
       <c r="B327" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E327">
         <v>53</v>
@@ -115888,7 +115888,7 @@
     <row r="328" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="1"/>
       <c r="B328" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E328">
         <v>3</v>
@@ -116230,7 +116230,7 @@
     <row r="329" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="1"/>
       <c r="B329" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C329">
         <v>1</v>
@@ -116608,7 +116608,7 @@
     <row r="330" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="B330" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E330">
         <v>10</v>
@@ -116974,7 +116974,7 @@
     <row r="331" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="B331" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F331">
         <v>319</v>
@@ -117301,7 +117301,7 @@
     <row r="332" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="B332" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E332">
         <v>2</v>
@@ -117622,7 +117622,7 @@
     <row r="333" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="1"/>
       <c r="B333" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F333">
         <v>49</v>
@@ -117898,7 +117898,7 @@
     <row r="334" spans="1:130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="B334" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E334">
         <v>3</v>

</xml_diff>